<commit_message>
Completed article on constant valued measure
</commit_message>
<xml_diff>
--- a/dax-constant-valued-measure/powerbi/DummySales.xlsx
+++ b/dax-constant-valued-measure/powerbi/DummySales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saurabhd\MyTrials\MyGithubPage\dax-constant-valued-measure\powerbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AEE474-76CE-4829-BC80-FEAAD90DFF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594072C1-9D62-4FBF-938D-9B66D7582474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54577794-3ED7-4157-AADF-842CD59B2D13}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>Adam</t>
   </si>
   <si>
-    <t>Smith1</t>
+    <t>Smith</t>
   </si>
 </sst>
 </file>

</xml_diff>